<commit_message>
+new quiz 2 images
</commit_message>
<xml_diff>
--- a/ref/quiz2.xlsx
+++ b/ref/quiz2.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khang\Desktop\webpages\rmcards\ref\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="15960" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
   <si>
     <t>arc pacis augustae</t>
   </si>
@@ -215,6 +220,42 @@
   </si>
   <si>
     <t>quiz2/16.png</t>
+  </si>
+  <si>
+    <t>forum of trajan</t>
+  </si>
+  <si>
+    <t>hadrian bust</t>
+  </si>
+  <si>
+    <t>panteon</t>
+  </si>
+  <si>
+    <t>column of marcus</t>
+  </si>
+  <si>
+    <t>112 ce</t>
+  </si>
+  <si>
+    <t>117-120 ce</t>
+  </si>
+  <si>
+    <t>118-125 ce</t>
+  </si>
+  <si>
+    <t>180-192 ce</t>
+  </si>
+  <si>
+    <t>quiz2/17.png</t>
+  </si>
+  <si>
+    <t>quiz2/18.png</t>
+  </si>
+  <si>
+    <t>quiz2/19.png</t>
+  </si>
+  <si>
+    <t>quiz2/20.png</t>
   </si>
 </sst>
 </file>
@@ -261,6 +302,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -309,7 +353,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -344,7 +388,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -553,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -841,6 +885,74 @@
         <v>66</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>